<commit_message>
update data and code phobert day 08/08/2024
</commit_message>
<xml_diff>
--- a/Data/fake.xlsx
+++ b/Data/fake.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1546" uniqueCount="790">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1658" uniqueCount="847">
   <si>
     <t>date</t>
   </si>
@@ -36023,6 +36023,617 @@
     }
 ]</t>
   </si>
+  <si>
+    <t>https://www.facebook.com/profile.php?id=100071065767015</t>
+  </si>
+  <si>
+    <t>Cháy một loạt 21 chiếc xe điện phục vụ du lịch ở Hội An, nhiều nhân viên đã tử vong ÔI THƯƠNG QUÁ XEM MÀ RÙNG MÌNH 
+full video xem chi tiết dưới bình luận</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/groups/943533259394424/permalink/2015973708817035/</t>
+  </si>
+  <si>
+    <t>29/07/2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vĩnh biệt nữ ca sỹ nổi tiếng vừa qua đời ở tuổi 21
+XOT XA CHO SHOWBIT QUA
+THƯƠNG E </t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/groups/943533259394424/permalink/2016492942098445/</t>
+  </si>
+  <si>
+    <r>
+      <t>NGAY LÚC NÀY KINH HOÀNG: XE KHÁCH CH</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11.5"/>
+        <color rgb="FF050505"/>
+        <rFont val="Times New Roman"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Ở</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11.5"/>
+        <color rgb="FF050505"/>
+        <rFont val="Segoe UI Historic"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> 30 HÀNH KHÁCH B</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11.5"/>
+        <color rgb="FF050505"/>
+        <rFont val="Times New Roman"/>
+        <charset val="134"/>
+      </rPr>
+      <t>ố</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11.5"/>
+        <color rgb="FF050505"/>
+        <rFont val="Segoe UI Historic"/>
+        <charset val="134"/>
+      </rPr>
+      <t>c cháy ngùn ng</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11.5"/>
+        <color rgb="FF050505"/>
+        <rFont val="Times New Roman"/>
+        <charset val="134"/>
+      </rPr>
+      <t>ụ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11.5"/>
+        <color rgb="FF050505"/>
+        <rFont val="Segoe UI Historic"/>
+        <charset val="134"/>
+      </rPr>
+      <t>t Trên Cao T</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11.5"/>
+        <color rgb="FF050505"/>
+        <rFont val="Times New Roman"/>
+        <charset val="134"/>
+      </rPr>
+      <t>ố</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11.5"/>
+        <color rgb="FF050505"/>
+        <rFont val="Segoe UI Historic"/>
+        <charset val="134"/>
+      </rPr>
+      <t>c..
+N</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11.5"/>
+        <color rgb="FF050505"/>
+        <rFont val="Times New Roman"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Ằ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11.5"/>
+        <color rgb="FF050505"/>
+        <rFont val="Segoe UI Historic"/>
+        <charset val="134"/>
+      </rPr>
+      <t>M LA LI</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11.5"/>
+        <color rgb="FF050505"/>
+        <rFont val="Times New Roman"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Ệ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11.5"/>
+        <color rgb="FF050505"/>
+        <rFont val="Segoe UI Historic"/>
+        <charset val="134"/>
+      </rPr>
+      <t>T R</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11.5"/>
+        <color rgb="FF050505"/>
+        <rFont val="Times New Roman"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Ồ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11.5"/>
+        <color rgb="FF050505"/>
+        <rFont val="Segoe UI Historic"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">I </t>
+    </r>
+  </si>
+  <si>
+    <t>https://www.facebook.com/groups/943533259394424/permalink/2016610712086668/</t>
+  </si>
+  <si>
+    <t>30/07/2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quảng Ninh – nơi đau thương lạnh lẽo nhất lúc này: HÀNG LOẠT công nhân khai thác hầm lò đã …LA LIỆT RỒI
+XEM RÙNG MÌNH 
+CHI TIẾT DƯỚI BÌNH LUẬN </t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/groups/943533259394424/permalink/2016643395416733/</t>
+  </si>
+  <si>
+    <t>30/07/2026</t>
+  </si>
+  <si>
+    <t>Vụ chồng "xuống tay" khiến vợ "ra đi" ở Ninh Bình: 2 con nhỏ chứng kiến tất cả, ám ảnh tiếng la hét trong tuyệt vọng</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/groups/943533259394424/permalink/2016660418748364/</t>
+  </si>
+  <si>
+    <t>30/07/2027</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lê Thu Vân - Em gái 'thầy ông nội' Tịnh thất Bồng lai vừa tu vong khi đang ..Dấu chấm hết chính thức cho Tịnh Thất Bồng Lai
+ÔI TO CHUYỆN RỒI XEM MÀ RÙNG MÌNH </t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/groups/943533259394424/permalink/2016712105409862/</t>
+  </si>
+  <si>
+    <t>30/07/2028</t>
+  </si>
+  <si>
+    <t>Hang Sửng Sốt Quảng Ninh: Địa điểm NÓNG nhất lúc này
+LA LIỆT LUÔN RỒI PHONG TỎA LUÔN RỒI
+XEM RÙNG MÌNH</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/groups/943533259394424/permalink/2017500771997662/</t>
+  </si>
+  <si>
+    <t>30/07/2029</t>
+  </si>
+  <si>
+    <t>Vừa xong: ‘Con gái’ xinh như hoa của nghệ sĩ Hồng Vân qua đời đột ngột khiến ai cũng thương tiếc</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/groups/943533259394424/permalink/2017585675322505/</t>
+  </si>
+  <si>
+    <t>30/07/2030</t>
+  </si>
+  <si>
+    <r>
+      <t>C</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11.5"/>
+        <color rgb="FF050505"/>
+        <rFont val="Times New Roman"/>
+        <charset val="134"/>
+      </rPr>
+      <t>ậ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11.5"/>
+        <color rgb="FF050505"/>
+        <rFont val="Segoe UI Historic"/>
+        <charset val="134"/>
+      </rPr>
+      <t>u bé Th</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11.5"/>
+        <color rgb="FF050505"/>
+        <rFont val="Times New Roman"/>
+        <charset val="134"/>
+      </rPr>
+      <t>ầ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11.5"/>
+        <color rgb="FF050505"/>
+        <rFont val="Segoe UI Historic"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">n </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11.5"/>
+        <color rgb="FF050505"/>
+        <rFont val="Times New Roman"/>
+        <charset val="134"/>
+      </rPr>
+      <t>đồ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11.5"/>
+        <color rgb="FF050505"/>
+        <rFont val="Segoe UI Historic"/>
+        <charset val="134"/>
+      </rPr>
+      <t>ng tiên tri nói v</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11.5"/>
+        <color rgb="FF050505"/>
+        <rFont val="Times New Roman"/>
+        <charset val="134"/>
+      </rPr>
+      <t>ề</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11.5"/>
+        <color rgb="FF050505"/>
+        <rFont val="Segoe UI Historic"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> 6 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11.5"/>
+        <color rgb="FF050505"/>
+        <rFont val="Times New Roman"/>
+        <charset val="134"/>
+      </rPr>
+      <t>đ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11.5"/>
+        <color rgb="FF050505"/>
+        <rFont val="Segoe UI Historic"/>
+        <charset val="134"/>
+      </rPr>
+      <t>i</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11.5"/>
+        <color rgb="FF050505"/>
+        <rFont val="Times New Roman"/>
+        <charset val="134"/>
+      </rPr>
+      <t>ề</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11.5"/>
+        <color rgb="FF050505"/>
+        <rFont val="Segoe UI Historic"/>
+        <charset val="134"/>
+      </rPr>
+      <t>u x</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11.5"/>
+        <color rgb="FF050505"/>
+        <rFont val="Times New Roman"/>
+        <charset val="134"/>
+      </rPr>
+      <t>ả</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11.5"/>
+        <color rgb="FF050505"/>
+        <rFont val="Segoe UI Historic"/>
+        <charset val="134"/>
+      </rPr>
+      <t>y ra v</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11.5"/>
+        <color rgb="FF050505"/>
+        <rFont val="Times New Roman"/>
+        <charset val="134"/>
+      </rPr>
+      <t>ớ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11.5"/>
+        <color rgb="FF050505"/>
+        <rFont val="Segoe UI Historic"/>
+        <charset val="134"/>
+      </rPr>
+      <t>i con ng</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11.5"/>
+        <color rgb="FF050505"/>
+        <rFont val="Times New Roman"/>
+        <charset val="134"/>
+      </rPr>
+      <t>ườ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11.5"/>
+        <color rgb="FF050505"/>
+        <rFont val="Segoe UI Historic"/>
+        <charset val="134"/>
+      </rPr>
+      <t>i n</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11.5"/>
+        <color rgb="FF050505"/>
+        <rFont val="Times New Roman"/>
+        <charset val="134"/>
+      </rPr>
+      <t>ă</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11.5"/>
+        <color rgb="FF050505"/>
+        <rFont val="Segoe UI Historic"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">m 2024, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11.5"/>
+        <color rgb="FF050505"/>
+        <rFont val="Times New Roman"/>
+        <charset val="134"/>
+      </rPr>
+      <t>đ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11.5"/>
+        <color rgb="FF050505"/>
+        <rFont val="Segoe UI Historic"/>
+        <charset val="134"/>
+      </rPr>
+      <t>i</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11.5"/>
+        <color rgb="FF050505"/>
+        <rFont val="Times New Roman"/>
+        <charset val="134"/>
+      </rPr>
+      <t>ề</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11.5"/>
+        <color rgb="FF050505"/>
+        <rFont val="Segoe UI Historic"/>
+        <charset val="134"/>
+      </rPr>
+      <t>u cu</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11.5"/>
+        <color rgb="FF050505"/>
+        <rFont val="Times New Roman"/>
+        <charset val="134"/>
+      </rPr>
+      <t>ố</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11.5"/>
+        <color rgb="FF050505"/>
+        <rFont val="Segoe UI Historic"/>
+        <charset val="134"/>
+      </rPr>
+      <t>i cùng khi</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11.5"/>
+        <color rgb="FF050505"/>
+        <rFont val="Times New Roman"/>
+        <charset val="134"/>
+      </rPr>
+      <t>ế</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11.5"/>
+        <color rgb="FF050505"/>
+        <rFont val="Segoe UI Historic"/>
+        <charset val="134"/>
+      </rPr>
+      <t>n nhi</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11.5"/>
+        <color rgb="FF050505"/>
+        <rFont val="Times New Roman"/>
+        <charset val="134"/>
+      </rPr>
+      <t>ề</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11.5"/>
+        <color rgb="FF050505"/>
+        <rFont val="Segoe UI Historic"/>
+        <charset val="134"/>
+      </rPr>
+      <t>u ng</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11.5"/>
+        <color rgb="FF050505"/>
+        <rFont val="Times New Roman"/>
+        <charset val="134"/>
+      </rPr>
+      <t>ườ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11.5"/>
+        <color rgb="FF050505"/>
+        <rFont val="Segoe UI Historic"/>
+        <charset val="134"/>
+      </rPr>
+      <t>i RÙNG MÌNH</t>
+    </r>
+  </si>
+  <si>
+    <t>https://www.facebook.com/groups/943533259394424/permalink/2017659938648412/</t>
+  </si>
+  <si>
+    <t>30/07/2031</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hiện trường kinh hoàng  xe tải cố vượt đường ray, khiến tàu hỏa trật bánh, vỡ nát: Ít nhất 100 người thương vong, hành khách hoảng loạn 
+XEM RÙNG MÌNH </t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/groups/943533259394424/permalink/2017906235290449/</t>
+  </si>
+  <si>
+    <t>Dự báo cơn bão lớn đen tối nhất của mùa bão 2024
+1 siêu bão mạnh chưa từng có cực kì đáng lo
+bà con lại khổ rồi</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/groups/943533259394424/permalink/2018681988546207/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SỐC RƠI CÁP TREO khiến 20 người tu vong tại chỗ 
+SỐC RƠI CÁP TREO khiến 20 người tu vong tại chỗ 
+SỐC RƠI CÁP TREO khiến 20 người tu vong tại chỗ 
+SỐC RƠI CÁP TREO khiến 20 người tu vong tại chỗ 
+</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/groups/943533259394424/permalink/2019110308503375/</t>
+  </si>
+  <si>
+    <t>30/07/2032</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bắc Kạn đau lòng nhất lúc này NẰM la liệt RỒI THƯƠNG LẮM BẮC CẠN ƠI </t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/groups/943533259394424/permalink/2019290375152035/</t>
+  </si>
+  <si>
+    <t>Cầu Long Biên: Địa điểm hot nhất lúc này?
+NẰM LA LIỆT RỒI 
+PHONG TỎA LUÔN RỒI</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/groups/943533259394424/permalink/2019330728481333/</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/profile.php?id=100058974272428</t>
+  </si>
+  <si>
+    <t>Vừa xong công an phong toả luôn rồi thương tâm quá</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/groups/943533259394424/permalink/1983769215370818/</t>
+  </si>
+  <si>
+    <t>Vừa xong,kinh hoàng quá, MÓNG CÁI nằm la liệt cả rồi
+ai là người nhà lên nhận đi</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/groups/943533259394424/permalink/1983575948723478/</t>
+  </si>
+  <si>
+    <t>Từ hôm nay người dân có thể mua vàng online
+GIÁ VÀNG CHOÁNG VÁNG</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/groups/943533259394424/permalink/1983494598731613/</t>
+  </si>
+  <si>
+    <t>NÓNG : KHÔNG CÒN AI XẾP HÀNG MUA VÀNG NỮA CHỈ VÌ....</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/groups/943533259394424/permalink/1983816602032746/</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> BIẾN CĂNG Ông chủ Salon tóc 1900 có động thái lạ
+SỰ THẬT PHƠI BÀY</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/groups/943533259394424/permalink/1984283268652746/</t>
+  </si>
+  <si>
+    <t>Động thái lạ của ông chủ salon 1900 trước nghi vấn ăn chặn 650 bộ tóc từ thiện cho bệnh nhân ung thư, những bộ tóc này đi về đâu?</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/groups/943533259394424/permalink/1984299608651112/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nghẹn lòng xót xa gia đình ông Thích Minh Tuệ nhận tin buồn lớn, người nhà ngày đêm túc trực trong viện chỉ mong sớm qua ‘kiếp nạn’
+THƯƠNG THẦY QUÁ </t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/groups/943533259394424/permalink/2019520211795718/</t>
+  </si>
+  <si>
+    <t>NGƯỜI DÂN XẾP HÀNG DÀI CHỜ XÉT NGHIỆM BẠCH HẦU</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/tintuc247247</t>
+  </si>
+  <si>
+    <t>vừa xong: tai nạn giao thông liên hoàn khiến 6 người thương vong</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/tintuc247247/posts/528530186395170?ref=embed_post</t>
+  </si>
 </sst>
 </file>
 
@@ -36034,7 +36645,7 @@
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="23">
+  <fonts count="25">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -36058,11 +36669,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
+      <sz val="11.5"/>
+      <color rgb="FF050505"/>
+      <name val="Segoe UI Historic"/>
       <charset val="134"/>
-      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11.25"/>
+      <color rgb="FF050505"/>
+      <name val="Segoe UI Historic"/>
+      <charset val="134"/>
     </font>
     <font>
       <u/>
@@ -36207,6 +36823,12 @@
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11.5"/>
+      <color rgb="FF050505"/>
+      <name val="Times New Roman"/>
+      <charset val="134"/>
     </font>
   </fonts>
   <fills count="33">
@@ -36542,16 +37164,13 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -36560,119 +37179,122 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -36701,7 +37323,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="58" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -37048,16 +37684,16 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:F309"/>
+  <dimension ref="A1:F332"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="A300" workbookViewId="0">
+      <selection activeCell="F333" sqref="F333"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" customHeight="1" outlineLevelCol="5"/>
   <cols>
-    <col min="1" max="1" width="9" style="2"/>
-    <col min="2" max="2" width="15.8148148148148" style="2" customWidth="1"/>
+    <col min="1" max="1" width="10.2222222222222" style="2"/>
+    <col min="2" max="2" width="36.1944444444444" style="2" customWidth="1"/>
     <col min="3" max="3" width="60.5185185185185" style="3" customWidth="1"/>
     <col min="4" max="4" width="9" style="2"/>
     <col min="5" max="5" width="19.0740740740741" style="2" customWidth="1"/>
@@ -43235,11 +43871,471 @@
       <c r="C309" s="10" t="s">
         <v>787</v>
       </c>
+      <c r="D309" s="2">
+        <v>0</v>
+      </c>
       <c r="E309" s="10" t="s">
         <v>788</v>
       </c>
       <c r="F309" s="10" t="s">
         <v>789</v>
+      </c>
+    </row>
+    <row r="310" customHeight="1" spans="1:6">
+      <c r="A310" s="2" t="s">
+        <v>432</v>
+      </c>
+      <c r="B310" s="2" t="s">
+        <v>790</v>
+      </c>
+      <c r="C310" s="11" t="s">
+        <v>791</v>
+      </c>
+      <c r="D310" s="2">
+        <v>0</v>
+      </c>
+      <c r="E310" s="2" t="s">
+        <v>792</v>
+      </c>
+      <c r="F310" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="311" customHeight="1" spans="1:6">
+      <c r="A311" s="2" t="s">
+        <v>793</v>
+      </c>
+      <c r="B311" s="2" t="s">
+        <v>790</v>
+      </c>
+      <c r="C311" s="11" t="s">
+        <v>794</v>
+      </c>
+      <c r="D311" s="2">
+        <v>0</v>
+      </c>
+      <c r="E311" s="2" t="s">
+        <v>795</v>
+      </c>
+      <c r="F311" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="312" customHeight="1" spans="1:6">
+      <c r="A312" s="2" t="s">
+        <v>435</v>
+      </c>
+      <c r="B312" s="2" t="s">
+        <v>790</v>
+      </c>
+      <c r="C312" s="12" t="s">
+        <v>796</v>
+      </c>
+      <c r="D312" s="2">
+        <v>0</v>
+      </c>
+      <c r="E312" s="2" t="s">
+        <v>797</v>
+      </c>
+      <c r="F312" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="313" customHeight="1" spans="1:6">
+      <c r="A313" s="2" t="s">
+        <v>798</v>
+      </c>
+      <c r="B313" s="2" t="s">
+        <v>790</v>
+      </c>
+      <c r="C313" s="13" t="s">
+        <v>799</v>
+      </c>
+      <c r="D313" s="2">
+        <v>0</v>
+      </c>
+      <c r="E313" s="2" t="s">
+        <v>800</v>
+      </c>
+      <c r="F313" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="314" customHeight="1" spans="1:6">
+      <c r="A314" s="2" t="s">
+        <v>801</v>
+      </c>
+      <c r="B314" s="2" t="s">
+        <v>790</v>
+      </c>
+      <c r="C314" s="3" t="s">
+        <v>802</v>
+      </c>
+      <c r="D314" s="2">
+        <v>0</v>
+      </c>
+      <c r="E314" s="2" t="s">
+        <v>803</v>
+      </c>
+      <c r="F314" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="315" customHeight="1" spans="1:6">
+      <c r="A315" s="2" t="s">
+        <v>804</v>
+      </c>
+      <c r="B315" s="2" t="s">
+        <v>790</v>
+      </c>
+      <c r="C315" s="13" t="s">
+        <v>805</v>
+      </c>
+      <c r="D315" s="2">
+        <v>0</v>
+      </c>
+      <c r="E315" s="2" t="s">
+        <v>806</v>
+      </c>
+      <c r="F315" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="316" customHeight="1" spans="1:6">
+      <c r="A316" s="2" t="s">
+        <v>807</v>
+      </c>
+      <c r="B316" s="2" t="s">
+        <v>790</v>
+      </c>
+      <c r="C316" s="13" t="s">
+        <v>808</v>
+      </c>
+      <c r="D316" s="2">
+        <v>0</v>
+      </c>
+      <c r="E316" s="2" t="s">
+        <v>809</v>
+      </c>
+      <c r="F316" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="317" customHeight="1" spans="1:6">
+      <c r="A317" s="2" t="s">
+        <v>810</v>
+      </c>
+      <c r="B317" s="2" t="s">
+        <v>790</v>
+      </c>
+      <c r="C317" s="3" t="s">
+        <v>811</v>
+      </c>
+      <c r="D317" s="2">
+        <v>0</v>
+      </c>
+      <c r="E317" s="2" t="s">
+        <v>812</v>
+      </c>
+      <c r="F317" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="318" customHeight="1" spans="1:6">
+      <c r="A318" s="2" t="s">
+        <v>813</v>
+      </c>
+      <c r="B318" s="2" t="s">
+        <v>790</v>
+      </c>
+      <c r="C318" s="14" t="s">
+        <v>814</v>
+      </c>
+      <c r="D318" s="2">
+        <v>0</v>
+      </c>
+      <c r="E318" s="2" t="s">
+        <v>815</v>
+      </c>
+      <c r="F318" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="319" customHeight="1" spans="1:6">
+      <c r="A319" s="2" t="s">
+        <v>816</v>
+      </c>
+      <c r="B319" s="2" t="s">
+        <v>790</v>
+      </c>
+      <c r="C319" s="13" t="s">
+        <v>817</v>
+      </c>
+      <c r="D319" s="2">
+        <v>0</v>
+      </c>
+      <c r="E319" s="2" t="s">
+        <v>818</v>
+      </c>
+      <c r="F319" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="320" customHeight="1" spans="2:6">
+      <c r="B320" s="2" t="s">
+        <v>790</v>
+      </c>
+      <c r="C320" s="13" t="s">
+        <v>819</v>
+      </c>
+      <c r="D320" s="2">
+        <v>0</v>
+      </c>
+      <c r="E320" s="2" t="s">
+        <v>820</v>
+      </c>
+      <c r="F320" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="321" customHeight="1" spans="1:6">
+      <c r="A321" s="15">
+        <v>45330</v>
+      </c>
+      <c r="B321" s="2" t="s">
+        <v>790</v>
+      </c>
+      <c r="C321" s="13" t="s">
+        <v>821</v>
+      </c>
+      <c r="D321" s="2">
+        <v>0</v>
+      </c>
+      <c r="E321" s="2" t="s">
+        <v>822</v>
+      </c>
+      <c r="F321" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="322" customHeight="1" spans="1:6">
+      <c r="A322" s="2" t="s">
+        <v>823</v>
+      </c>
+      <c r="B322" s="2" t="s">
+        <v>790</v>
+      </c>
+      <c r="C322" s="3" t="s">
+        <v>824</v>
+      </c>
+      <c r="D322" s="2">
+        <v>0</v>
+      </c>
+      <c r="E322" s="2" t="s">
+        <v>825</v>
+      </c>
+      <c r="F322" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="323" customHeight="1" spans="1:6">
+      <c r="A323" s="2" t="s">
+        <v>823</v>
+      </c>
+      <c r="B323" s="2" t="s">
+        <v>790</v>
+      </c>
+      <c r="C323" s="13" t="s">
+        <v>826</v>
+      </c>
+      <c r="D323" s="2">
+        <v>0</v>
+      </c>
+      <c r="E323" s="2" t="s">
+        <v>827</v>
+      </c>
+      <c r="F323" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="324" customHeight="1" spans="1:6">
+      <c r="A324" s="2" t="s">
+        <v>823</v>
+      </c>
+      <c r="B324" s="2" t="s">
+        <v>828</v>
+      </c>
+      <c r="C324" s="3" t="s">
+        <v>829</v>
+      </c>
+      <c r="D324" s="2">
+        <v>0</v>
+      </c>
+      <c r="E324" s="2" t="s">
+        <v>830</v>
+      </c>
+      <c r="F324" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="325" customHeight="1" spans="1:6">
+      <c r="A325" s="2" t="s">
+        <v>823</v>
+      </c>
+      <c r="B325" s="2" t="s">
+        <v>828</v>
+      </c>
+      <c r="C325" s="13" t="s">
+        <v>831</v>
+      </c>
+      <c r="D325" s="2">
+        <v>0</v>
+      </c>
+      <c r="E325" s="2" t="s">
+        <v>832</v>
+      </c>
+      <c r="F325" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="326" customHeight="1" spans="1:6">
+      <c r="A326" s="2" t="s">
+        <v>823</v>
+      </c>
+      <c r="B326" s="2" t="s">
+        <v>828</v>
+      </c>
+      <c r="C326" s="13" t="s">
+        <v>833</v>
+      </c>
+      <c r="D326" s="2">
+        <v>0</v>
+      </c>
+      <c r="E326" s="2" t="s">
+        <v>834</v>
+      </c>
+      <c r="F326" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="327" customHeight="1" spans="1:6">
+      <c r="A327" s="2" t="s">
+        <v>823</v>
+      </c>
+      <c r="B327" s="2" t="s">
+        <v>828</v>
+      </c>
+      <c r="C327" s="3" t="s">
+        <v>835</v>
+      </c>
+      <c r="D327" s="2">
+        <v>0</v>
+      </c>
+      <c r="E327" s="2" t="s">
+        <v>836</v>
+      </c>
+      <c r="F327" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="328" customHeight="1" spans="1:6">
+      <c r="A328" s="2" t="s">
+        <v>823</v>
+      </c>
+      <c r="B328" s="2" t="s">
+        <v>828</v>
+      </c>
+      <c r="C328" s="13" t="s">
+        <v>837</v>
+      </c>
+      <c r="D328" s="2">
+        <v>0</v>
+      </c>
+      <c r="E328" s="2" t="s">
+        <v>838</v>
+      </c>
+      <c r="F328" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="329" customHeight="1" spans="1:6">
+      <c r="A329" s="2" t="s">
+        <v>823</v>
+      </c>
+      <c r="B329" s="2" t="s">
+        <v>828</v>
+      </c>
+      <c r="C329" s="3" t="s">
+        <v>839</v>
+      </c>
+      <c r="D329" s="2">
+        <v>0</v>
+      </c>
+      <c r="E329" s="2" t="s">
+        <v>840</v>
+      </c>
+      <c r="F329" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="330" customHeight="1" spans="1:6">
+      <c r="A330" s="2" t="s">
+        <v>823</v>
+      </c>
+      <c r="B330" s="2" t="s">
+        <v>828</v>
+      </c>
+      <c r="C330" s="13" t="s">
+        <v>841</v>
+      </c>
+      <c r="D330" s="2">
+        <v>0</v>
+      </c>
+      <c r="E330" s="2" t="s">
+        <v>842</v>
+      </c>
+      <c r="F330" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="331" customHeight="1" spans="1:6">
+      <c r="A331" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B331" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C331" s="16" t="s">
+        <v>843</v>
+      </c>
+      <c r="D331" s="2">
+        <v>0</v>
+      </c>
+      <c r="E331" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F331" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="332" customHeight="1" spans="1:6">
+      <c r="A332" s="15">
+        <v>45481</v>
+      </c>
+      <c r="B332" s="2" t="s">
+        <v>844</v>
+      </c>
+      <c r="C332" s="3" t="s">
+        <v>845</v>
+      </c>
+      <c r="D332" s="2">
+        <v>0</v>
+      </c>
+      <c r="E332" s="2" t="s">
+        <v>846</v>
+      </c>
+      <c r="F332" s="2" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>